<commit_message>
Diagrama de Event Stormin
</commit_message>
<xml_diff>
--- a/HojaVidaComputo/UbicacionesInstitucion - MuestreoDatos.xlsx
+++ b/HojaVidaComputo/UbicacionesInstitucion - MuestreoDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\HojaVidaComputo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/HojaVidaComputo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0C2268-711F-40E1-A1D8-0E6D20FA259C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{9B0C2268-711F-40E1-A1D8-0E6D20FA259C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC44EF5D-17AA-465A-BA85-2AA3D15C4727}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="11" xr2:uid="{85AF6D48-FDD5-4A15-BC1B-8DA82DA63D0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{85AF6D48-FDD5-4A15-BC1B-8DA82DA63D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>Objeto de dominio que representa a cada una de las ubicaciones de la institucion donde existe computadores</t>
   </si>
   <si>
-    <t>Ubicaciones Institucion</t>
-  </si>
-  <si>
     <t>Sala Computo 1</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>Avenida estelar cerca al supermecado la gloria</t>
+  </si>
+  <si>
+    <t>Ubicaciones Sedes Institucion</t>
   </si>
 </sst>
 </file>
@@ -435,23 +435,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>534325</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>524762</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>134087</xdr:rowOff>
+      <xdr:rowOff>10224</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3357D8C0-1079-53EF-530B-369A8A068F4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8307B3E-42C3-6125-5B88-14817C5B735C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -467,8 +467,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="381000"/>
-          <a:ext cx="6630325" cy="5277587"/>
+          <a:off x="266700" y="523875"/>
+          <a:ext cx="6354062" cy="5010849"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB2B1D3-F4EF-49F9-AFA2-1ECC5999F861}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -880,35 +880,35 @@
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -916,83 +916,83 @@
         <v>13</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -1037,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1100,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
         <v>33042</v>
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1173,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>Pais!C3</f>
@@ -1189,7 +1189,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>Pais!C4</f>
@@ -1209,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAEF0ED-089F-46A1-8990-418DB8F9F740}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="str">
         <f>B2</f>
@@ -1241,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C4" si="0">B3</f>
@@ -1253,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1291,7 +1291,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>2</v>
@@ -1302,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>TipoUbicacion!D5</f>
@@ -1322,7 +1322,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6" t="str">
         <f>TipoUbicacion!D2</f>
@@ -1342,7 +1342,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="str">
         <f>TipoUbicacion!D5</f>
@@ -1366,7 +1366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C164FFC4-9C67-429F-A92C-ED12673A1B6E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -1432,7 +1432,7 @@
         <v>900810300-NIT</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="str">
         <f t="shared" ref="D3:D5" si="0">B3&amp;"-"&amp;C3</f>
@@ -1448,7 +1448,7 @@
         <v>900810200-RUT</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="str">
         <f>B2</f>
@@ -1520,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C5" si="0">B3</f>
@@ -1532,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1544,7 +1544,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1585,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5" t="str">
         <f>B2</f>
@@ -1597,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C5" si="0">B3</f>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="str">
         <f>B2</f>
@@ -1672,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C4" si="0">B3</f>
@@ -1684,7 +1684,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1719,22 +1719,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1758,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="7" t="str">
         <f>TipoInstitucion!C3</f>
@@ -1792,7 +1792,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7" t="str">
         <f>TipoInstitucion!C4</f>
@@ -1826,7 +1826,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="7" t="str">
         <f>TipoInstitucion!C5</f>
@@ -1890,16 +1890,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>2</v>
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>TipoSede!C2</f>
@@ -1925,7 +1925,7 @@
         <v>Rionegro-Antioquia-Colombia</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="5" t="str">
         <f>B2&amp;"-"&amp;C2&amp;"-"&amp;E2&amp;"-"&amp;F2</f>
@@ -1937,7 +1937,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>TipoSede!C3</f>
@@ -1952,7 +1952,7 @@
         <v>Medellin-Santander-Usa</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G4" si="0">B3&amp;"-"&amp;C3&amp;"-"&amp;E3&amp;"-"&amp;F3</f>
@@ -1964,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>TipoSede!C2</f>
@@ -1979,7 +1979,7 @@
         <v>Marinilla-Cundinamarca-España</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="str">
         <f>B2</f>
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3" si="0">B3</f>
@@ -2045,23 +2045,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c0fdd826-2c97-4883-aa16-15e3c35e6b68" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B6BB312010404D449723FB359E67F8CE" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="21adac9698eeb849927f810cac50c5aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c0fdd826-2c97-4883-aa16-15e3c35e6b68" xmlns:ns4="78d03883-3f22-4885-97bf-a69f9aeef276" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e45149a19d303b1813e3382f63f0e34e" ns3:_="" ns4:_="">
     <xsd:import namespace="c0fdd826-2c97-4883-aa16-15e3c35e6b68"/>
@@ -2300,32 +2283,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c0fdd826-2c97-4883-aa16-15e3c35e6b68" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C313C4-4138-4250-8E4E-11ABED0F2AFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c0fdd826-2c97-4883-aa16-15e3c35e6b68"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="78d03883-3f22-4885-97bf-a69f9aeef276"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91ACFA37-F4E1-4C13-8AC5-ED947B7B8D38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A081A1B6-BDB6-4746-8B29-8B33BCC3FB81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2342,4 +2317,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91ACFA37-F4E1-4C13-8AC5-ED947B7B8D38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C313C4-4138-4250-8E4E-11ABED0F2AFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c0fdd826-2c97-4883-aa16-15e3c35e6b68"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="78d03883-3f22-4885-97bf-a69f9aeef276"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>